<commit_message>
added unit tests for Joe Model
</commit_message>
<xml_diff>
--- a/inst/stressor-response_fixed_ARTR.xlsx
+++ b/inst/stressor-response_fixed_ARTR.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24729"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654832CC-6737-49D5-88AC-A3D0E30639F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18D85110-7870-4B47-849F-3932B125E6BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2820" yWindow="12492" windowWidth="23256" windowHeight="12576" firstSheet="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22932" yWindow="2052" windowWidth="23256" windowHeight="12576" firstSheet="6" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="2" r:id="rId1"/>
@@ -15042,8 +15042,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -16016,8 +16016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>